<commit_message>
WebEdit initialized constructor ComboBox initialized constructor Webtable initialized constructor Webtable insert data to new row(hashtable/array) Webtable insert data to new row(hashtable/array) inputData to hashtable/array
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationSelenuim\seleniumaf\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationSelenuim\scout_demo\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -50,46 +50,22 @@
     <t>a</t>
   </si>
   <si>
-    <t>LogIn Alis 3</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>LogIn Alis 4</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>LogIn Alis 5</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>LogIn Alis 6</t>
-  </si>
-  <si>
-    <t>a5</t>
-  </si>
-  <si>
     <t>tfl_6631_auto</t>
   </si>
   <si>
     <t>DataBase</t>
   </si>
   <si>
-    <t>http://alis-alf-app01:8080/af_pl_env1/alis1#alis</t>
-  </si>
-  <si>
-    <t>af_7000_defs</t>
-  </si>
-  <si>
     <t>LogIn Alis TFL</t>
   </si>
   <si>
     <t>LogIn Alis AF</t>
+  </si>
+  <si>
+    <t>http://alis-alf-app01:8082/af_pl_env2/alis#alis</t>
+  </si>
+  <si>
+    <t>af_7000_michael</t>
   </si>
 </sst>
 </file>
@@ -472,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -512,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -524,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -532,10 +508,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -544,94 +520,11 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
         <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" location="alis" display="http://alis-alf-app01:8080/af_pl_env1/alis1 - alis"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>